<commit_message>
Updated projects with pictures
</commit_message>
<xml_diff>
--- a/Personal Website Projects.xlsx
+++ b/Personal Website Projects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin Chang\Drive\Professional\2020 Job Search\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin Chang\Drive\Professional\Personal Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89E7D1A-5434-47B6-8C93-1EC1A456133A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1687976-A725-40DB-94C4-07E24D461AF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22095" yWindow="570" windowWidth="13890" windowHeight="14715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Project</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>images, push code to github, link to paper</t>
+  </si>
+  <si>
+    <t>Maybe some cool analysis project</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,6 +583,11 @@
         <v>25</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated project images with 500px width
</commit_message>
<xml_diff>
--- a/Personal Website Projects.xlsx
+++ b/Personal Website Projects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin Chang\Drive\Professional\Personal Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1687976-A725-40DB-94C4-07E24D461AF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F87E3B-C3DB-4763-9611-4A5DF6DBC8C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Project</t>
   </si>
@@ -45,21 +45,12 @@
     <t>TEG</t>
   </si>
   <si>
-    <t>BARC, QUAD</t>
-  </si>
-  <si>
     <t>OLLY</t>
   </si>
   <si>
-    <t>SMV CFD</t>
-  </si>
-  <si>
     <t>Movi Pro</t>
   </si>
   <si>
-    <t>SMV Powertrain, Battery</t>
-  </si>
-  <si>
     <t>3D Printing Adventures</t>
   </si>
   <si>
@@ -69,21 +60,12 @@
     <t>CS 170 Project</t>
   </si>
   <si>
-    <t>ansys results, images</t>
-  </si>
-  <si>
     <t>poster board, images, block diagram, analysis results</t>
   </si>
   <si>
-    <t>images, videos, simulink block diagram, code push to github</t>
-  </si>
-  <si>
     <t>github</t>
   </si>
   <si>
-    <t>final video</t>
-  </si>
-  <si>
     <t>Maplab</t>
   </si>
   <si>
@@ -114,13 +96,37 @@
     <t>images, simulink block diagram, video</t>
   </si>
   <si>
-    <t>images, CAD, etc, brochure</t>
-  </si>
-  <si>
     <t>images, push code to github, link to paper</t>
   </si>
   <si>
     <t>Maybe some cool analysis project</t>
+  </si>
+  <si>
+    <t>C180 FEM Projects</t>
+  </si>
+  <si>
+    <t>E7 Marching Project</t>
+  </si>
+  <si>
+    <t>Drifting, images, videos, simulink block diagram, code push to github</t>
+  </si>
+  <si>
+    <t>Quadcopter 136</t>
+  </si>
+  <si>
+    <t>BARC 131</t>
+  </si>
+  <si>
+    <t>final video, CAD, link to movipro</t>
+  </si>
+  <si>
+    <t>images, CAD, etc, brochure, ansys results, images</t>
+  </si>
+  <si>
+    <t>SMV Powertrain, Battery, CFD</t>
+  </si>
+  <si>
+    <t>Code, images, videos</t>
   </si>
 </sst>
 </file>
@@ -447,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,10 +479,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -484,7 +490,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -492,100 +498,108 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>31</v>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>